<commit_message>
Update latest document and source
</commit_message>
<xml_diff>
--- a/01_Documents/Message_List_20180321.xlsx
+++ b/01_Documents/Message_List_20180321.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="44">
   <si>
     <t>#</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>Expand Data</t>
+  </si>
+  <si>
+    <t>check_moderator</t>
+  </si>
+  <si>
+    <t>get_content</t>
   </si>
 </sst>
 </file>
@@ -489,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -506,6 +512,18 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -542,9 +560,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,7 +864,7 @@
   <dimension ref="A1:U52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -887,27 +902,27 @@
       <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="19" t="s">
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="21"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="27"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
@@ -934,15 +949,15 @@
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
       <c r="P3" s="10"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="24"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="30"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
@@ -979,15 +994,15 @@
         <v>14</v>
       </c>
       <c r="L4" s="15"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
       <c r="P4" s="14"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="18"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="24"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
@@ -1014,15 +1029,15 @@
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
       <c r="P5" s="14"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="18"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="24"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
@@ -1047,15 +1062,15 @@
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
       <c r="P6" s="14"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="18"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="24"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
@@ -1082,15 +1097,15 @@
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
       <c r="L7" s="15"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
       <c r="P7" s="14"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="18"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="24"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
@@ -1115,15 +1130,15 @@
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
       <c r="P8" s="14"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="18"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="24"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
@@ -1158,15 +1173,15 @@
       </c>
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
       <c r="P9" s="14"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="18"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="24"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
@@ -1191,15 +1206,15 @@
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
       <c r="P10" s="14"/>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
-      <c r="U10" s="18"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="24"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
@@ -1226,15 +1241,15 @@
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
       <c r="P11" s="14"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="18"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="24"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
@@ -1259,25 +1274,25 @@
       <c r="J12" s="15"/>
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
       <c r="P12" s="14"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="17"/>
-      <c r="S12" s="17"/>
-      <c r="T12" s="17"/>
-      <c r="U12" s="18"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="24"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>11</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>6</v>
@@ -1292,28 +1307,28 @@
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
       <c r="P13" s="14"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="17"/>
-      <c r="U13" s="18"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
+      <c r="U13" s="24"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>12</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>15</v>
@@ -1325,22 +1340,22 @@
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
       <c r="P14" s="14"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="17"/>
-      <c r="U14" s="18"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23"/>
+      <c r="T14" s="23"/>
+      <c r="U14" s="24"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>13</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>22</v>
@@ -1352,7 +1367,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
@@ -1360,22 +1375,22 @@
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
       <c r="P15" s="14"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="17"/>
-      <c r="U15" s="18"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="24"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>14</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>6</v>
@@ -1393,25 +1408,25 @@
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="29"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
       <c r="P16" s="14"/>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
-      <c r="T16" s="17"/>
-      <c r="U16" s="18"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="24"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>15</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>6</v>
@@ -1419,16 +1434,18 @@
       <c r="E17" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="15"/>
+      <c r="F17" s="15" t="s">
+        <v>24</v>
+      </c>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="29"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
       <c r="P17" s="14"/>
       <c r="Q17" s="16"/>
       <c r="R17" s="17"/>
@@ -1441,29 +1458,27 @@
         <v>16</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="15" t="s">
-        <v>26</v>
-      </c>
+      <c r="F18" s="15"/>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="29"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
       <c r="P18" s="14"/>
       <c r="Q18" s="16"/>
       <c r="R18" s="17"/>
@@ -1476,31 +1491,25 @@
         <v>17</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="29"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
       <c r="P19" s="14"/>
       <c r="Q19" s="16"/>
       <c r="R19" s="17"/>
@@ -1513,27 +1522,29 @@
         <v>18</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="15"/>
+      <c r="F20" s="15" t="s">
+        <v>26</v>
+      </c>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
       <c r="L20" s="15"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="29"/>
-      <c r="O20" s="29"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
       <c r="P20" s="14"/>
       <c r="Q20" s="16"/>
       <c r="R20" s="17"/>
@@ -1546,10 +1557,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>6</v>
@@ -1560,15 +1571,17 @@
       <c r="F21" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="15"/>
+      <c r="G21" s="15" t="s">
+        <v>29</v>
+      </c>
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
       <c r="L21" s="15"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="29"/>
-      <c r="O21" s="29"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="20"/>
       <c r="P21" s="14"/>
       <c r="Q21" s="16"/>
       <c r="R21" s="17"/>
@@ -1581,29 +1594,27 @@
         <v>20</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="E22" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="15" t="s">
-        <v>31</v>
-      </c>
+      <c r="F22" s="15"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
       <c r="L22" s="15"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="29"/>
-      <c r="O22" s="29"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
       <c r="P22" s="14"/>
       <c r="Q22" s="16"/>
       <c r="R22" s="17"/>
@@ -1616,7 +1627,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>5</v>
@@ -1625,41 +1636,19 @@
         <v>6</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="J23" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="K23" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="L23" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="M23" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="N23" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="O23" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="P23" s="14" t="s">
-        <v>41</v>
-      </c>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="14"/>
       <c r="Q23" s="16"/>
       <c r="R23" s="17"/>
       <c r="S23" s="17"/>
@@ -1671,7 +1660,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>6</v>
@@ -1682,16 +1671,18 @@
       <c r="E24" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F24" s="15"/>
+      <c r="F24" s="15" t="s">
+        <v>31</v>
+      </c>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
       <c r="K24" s="15"/>
       <c r="L24" s="15"/>
-      <c r="M24" s="29"/>
-      <c r="N24" s="29"/>
-      <c r="O24" s="29"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="20"/>
       <c r="P24" s="14"/>
       <c r="Q24" s="16"/>
       <c r="R24" s="17"/>
@@ -1703,21 +1694,51 @@
       <c r="A25" s="12">
         <v>23</v>
       </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="29"/>
-      <c r="N25" s="29"/>
-      <c r="O25" s="29"/>
-      <c r="P25" s="14"/>
+      <c r="B25" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J25" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K25" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L25" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="M25" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="N25" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="O25" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="P25" s="14" t="s">
+        <v>41</v>
+      </c>
       <c r="Q25" s="16"/>
       <c r="R25" s="17"/>
       <c r="S25" s="17"/>
@@ -1728,10 +1749,18 @@
       <c r="A26" s="12">
         <v>24</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="13"/>
+      <c r="B26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>15</v>
+      </c>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
@@ -1739,9 +1768,9 @@
       <c r="J26" s="15"/>
       <c r="K26" s="15"/>
       <c r="L26" s="15"/>
-      <c r="M26" s="29"/>
-      <c r="N26" s="29"/>
-      <c r="O26" s="29"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="20"/>
       <c r="P26" s="14"/>
       <c r="Q26" s="16"/>
       <c r="R26" s="17"/>
@@ -1753,9 +1782,15 @@
       <c r="A27" s="12">
         <v>25</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="14"/>
+      <c r="B27" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>6</v>
+      </c>
       <c r="E27" s="13"/>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
@@ -1764,23 +1799,29 @@
       <c r="J27" s="15"/>
       <c r="K27" s="15"/>
       <c r="L27" s="15"/>
-      <c r="M27" s="29"/>
-      <c r="N27" s="29"/>
-      <c r="O27" s="29"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="20"/>
       <c r="P27" s="14"/>
-      <c r="Q27" s="16"/>
-      <c r="R27" s="17"/>
-      <c r="S27" s="17"/>
-      <c r="T27" s="17"/>
-      <c r="U27" s="18"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="23"/>
+      <c r="S27" s="23"/>
+      <c r="T27" s="23"/>
+      <c r="U27" s="24"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>26</v>
       </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="14"/>
+      <c r="B28" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>5</v>
+      </c>
       <c r="E28" s="13"/>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
@@ -1789,15 +1830,15 @@
       <c r="J28" s="15"/>
       <c r="K28" s="15"/>
       <c r="L28" s="15"/>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29"/>
-      <c r="O28" s="29"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="20"/>
       <c r="P28" s="14"/>
-      <c r="Q28" s="16"/>
-      <c r="R28" s="17"/>
-      <c r="S28" s="17"/>
-      <c r="T28" s="17"/>
-      <c r="U28" s="18"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="23"/>
+      <c r="S28" s="23"/>
+      <c r="T28" s="23"/>
+      <c r="U28" s="24"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
@@ -1814,15 +1855,15 @@
       <c r="J29" s="15"/>
       <c r="K29" s="15"/>
       <c r="L29" s="15"/>
-      <c r="M29" s="29"/>
-      <c r="N29" s="29"/>
-      <c r="O29" s="29"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
       <c r="P29" s="14"/>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="17"/>
-      <c r="S29" s="17"/>
-      <c r="T29" s="17"/>
-      <c r="U29" s="18"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
+      <c r="T29" s="23"/>
+      <c r="U29" s="24"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
@@ -1839,15 +1880,15 @@
       <c r="J30" s="15"/>
       <c r="K30" s="15"/>
       <c r="L30" s="15"/>
-      <c r="M30" s="29"/>
-      <c r="N30" s="29"/>
-      <c r="O30" s="29"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
+      <c r="O30" s="20"/>
       <c r="P30" s="14"/>
-      <c r="Q30" s="16"/>
-      <c r="R30" s="17"/>
-      <c r="S30" s="17"/>
-      <c r="T30" s="17"/>
-      <c r="U30" s="18"/>
+      <c r="Q30" s="22"/>
+      <c r="R30" s="23"/>
+      <c r="S30" s="23"/>
+      <c r="T30" s="23"/>
+      <c r="U30" s="24"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
@@ -1864,15 +1905,15 @@
       <c r="J31" s="15"/>
       <c r="K31" s="15"/>
       <c r="L31" s="15"/>
-      <c r="M31" s="29"/>
-      <c r="N31" s="29"/>
-      <c r="O31" s="29"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
+      <c r="O31" s="20"/>
       <c r="P31" s="14"/>
-      <c r="Q31" s="16"/>
-      <c r="R31" s="17"/>
-      <c r="S31" s="17"/>
-      <c r="T31" s="17"/>
-      <c r="U31" s="18"/>
+      <c r="Q31" s="22"/>
+      <c r="R31" s="23"/>
+      <c r="S31" s="23"/>
+      <c r="T31" s="23"/>
+      <c r="U31" s="24"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
@@ -1889,15 +1930,15 @@
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
       <c r="L32" s="15"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
-      <c r="O32" s="29"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="20"/>
       <c r="P32" s="14"/>
-      <c r="Q32" s="16"/>
-      <c r="R32" s="17"/>
-      <c r="S32" s="17"/>
-      <c r="T32" s="17"/>
-      <c r="U32" s="18"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="23"/>
+      <c r="S32" s="23"/>
+      <c r="T32" s="23"/>
+      <c r="U32" s="24"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
@@ -1914,15 +1955,15 @@
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
       <c r="L33" s="15"/>
-      <c r="M33" s="29"/>
-      <c r="N33" s="29"/>
-      <c r="O33" s="29"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="20"/>
       <c r="P33" s="14"/>
-      <c r="Q33" s="16"/>
-      <c r="R33" s="17"/>
-      <c r="S33" s="17"/>
-      <c r="T33" s="17"/>
-      <c r="U33" s="18"/>
+      <c r="Q33" s="22"/>
+      <c r="R33" s="23"/>
+      <c r="S33" s="23"/>
+      <c r="T33" s="23"/>
+      <c r="U33" s="24"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
@@ -1939,15 +1980,15 @@
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
       <c r="L34" s="15"/>
-      <c r="M34" s="29"/>
-      <c r="N34" s="29"/>
-      <c r="O34" s="29"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="20"/>
+      <c r="O34" s="20"/>
       <c r="P34" s="14"/>
-      <c r="Q34" s="16"/>
-      <c r="R34" s="17"/>
-      <c r="S34" s="17"/>
-      <c r="T34" s="17"/>
-      <c r="U34" s="18"/>
+      <c r="Q34" s="22"/>
+      <c r="R34" s="23"/>
+      <c r="S34" s="23"/>
+      <c r="T34" s="23"/>
+      <c r="U34" s="24"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
@@ -1964,15 +2005,15 @@
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
       <c r="L35" s="15"/>
-      <c r="M35" s="29"/>
-      <c r="N35" s="29"/>
-      <c r="O35" s="29"/>
+      <c r="M35" s="20"/>
+      <c r="N35" s="20"/>
+      <c r="O35" s="20"/>
       <c r="P35" s="14"/>
-      <c r="Q35" s="16"/>
-      <c r="R35" s="17"/>
-      <c r="S35" s="17"/>
-      <c r="T35" s="17"/>
-      <c r="U35" s="18"/>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="23"/>
+      <c r="S35" s="23"/>
+      <c r="T35" s="23"/>
+      <c r="U35" s="24"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A36" s="12">
@@ -1989,15 +2030,15 @@
       <c r="J36" s="15"/>
       <c r="K36" s="15"/>
       <c r="L36" s="15"/>
-      <c r="M36" s="29"/>
-      <c r="N36" s="29"/>
-      <c r="O36" s="29"/>
+      <c r="M36" s="20"/>
+      <c r="N36" s="20"/>
+      <c r="O36" s="20"/>
       <c r="P36" s="14"/>
-      <c r="Q36" s="16"/>
-      <c r="R36" s="17"/>
-      <c r="S36" s="17"/>
-      <c r="T36" s="17"/>
-      <c r="U36" s="18"/>
+      <c r="Q36" s="22"/>
+      <c r="R36" s="23"/>
+      <c r="S36" s="23"/>
+      <c r="T36" s="23"/>
+      <c r="U36" s="24"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A37" s="12">
@@ -2014,15 +2055,15 @@
       <c r="J37" s="15"/>
       <c r="K37" s="15"/>
       <c r="L37" s="15"/>
-      <c r="M37" s="29"/>
-      <c r="N37" s="29"/>
-      <c r="O37" s="29"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="20"/>
       <c r="P37" s="14"/>
-      <c r="Q37" s="16"/>
-      <c r="R37" s="17"/>
-      <c r="S37" s="17"/>
-      <c r="T37" s="17"/>
-      <c r="U37" s="18"/>
+      <c r="Q37" s="22"/>
+      <c r="R37" s="23"/>
+      <c r="S37" s="23"/>
+      <c r="T37" s="23"/>
+      <c r="U37" s="24"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A38" s="12">
@@ -2039,15 +2080,15 @@
       <c r="J38" s="15"/>
       <c r="K38" s="15"/>
       <c r="L38" s="15"/>
-      <c r="M38" s="29"/>
-      <c r="N38" s="29"/>
-      <c r="O38" s="29"/>
+      <c r="M38" s="20"/>
+      <c r="N38" s="20"/>
+      <c r="O38" s="20"/>
       <c r="P38" s="14"/>
-      <c r="Q38" s="16"/>
-      <c r="R38" s="17"/>
-      <c r="S38" s="17"/>
-      <c r="T38" s="17"/>
-      <c r="U38" s="18"/>
+      <c r="Q38" s="22"/>
+      <c r="R38" s="23"/>
+      <c r="S38" s="23"/>
+      <c r="T38" s="23"/>
+      <c r="U38" s="24"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A39" s="12">
@@ -2064,15 +2105,15 @@
       <c r="J39" s="15"/>
       <c r="K39" s="15"/>
       <c r="L39" s="15"/>
-      <c r="M39" s="29"/>
-      <c r="N39" s="29"/>
-      <c r="O39" s="29"/>
+      <c r="M39" s="20"/>
+      <c r="N39" s="20"/>
+      <c r="O39" s="20"/>
       <c r="P39" s="14"/>
-      <c r="Q39" s="16"/>
-      <c r="R39" s="17"/>
-      <c r="S39" s="17"/>
-      <c r="T39" s="17"/>
-      <c r="U39" s="18"/>
+      <c r="Q39" s="22"/>
+      <c r="R39" s="23"/>
+      <c r="S39" s="23"/>
+      <c r="T39" s="23"/>
+      <c r="U39" s="24"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
@@ -2089,15 +2130,15 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
-      <c r="M40" s="30"/>
-      <c r="N40" s="30"/>
-      <c r="O40" s="30"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="21"/>
       <c r="P40" s="4"/>
-      <c r="Q40" s="25"/>
-      <c r="R40" s="26"/>
-      <c r="S40" s="26"/>
-      <c r="T40" s="26"/>
-      <c r="U40" s="27"/>
+      <c r="Q40" s="31"/>
+      <c r="R40" s="32"/>
+      <c r="S40" s="32"/>
+      <c r="T40" s="32"/>
+      <c r="U40" s="33"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
@@ -2114,15 +2155,15 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
-      <c r="M41" s="30"/>
-      <c r="N41" s="30"/>
-      <c r="O41" s="30"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
+      <c r="O41" s="21"/>
       <c r="P41" s="4"/>
-      <c r="Q41" s="25"/>
-      <c r="R41" s="26"/>
-      <c r="S41" s="26"/>
-      <c r="T41" s="26"/>
-      <c r="U41" s="27"/>
+      <c r="Q41" s="31"/>
+      <c r="R41" s="32"/>
+      <c r="S41" s="32"/>
+      <c r="T41" s="32"/>
+      <c r="U41" s="33"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
@@ -2139,15 +2180,15 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
-      <c r="M42" s="30"/>
-      <c r="N42" s="30"/>
-      <c r="O42" s="30"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="21"/>
       <c r="P42" s="4"/>
-      <c r="Q42" s="25"/>
-      <c r="R42" s="26"/>
-      <c r="S42" s="26"/>
-      <c r="T42" s="26"/>
-      <c r="U42" s="27"/>
+      <c r="Q42" s="31"/>
+      <c r="R42" s="32"/>
+      <c r="S42" s="32"/>
+      <c r="T42" s="32"/>
+      <c r="U42" s="33"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
@@ -2164,15 +2205,15 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
-      <c r="M43" s="30"/>
-      <c r="N43" s="30"/>
-      <c r="O43" s="30"/>
+      <c r="M43" s="21"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="21"/>
       <c r="P43" s="4"/>
-      <c r="Q43" s="25"/>
-      <c r="R43" s="26"/>
-      <c r="S43" s="26"/>
-      <c r="T43" s="26"/>
-      <c r="U43" s="27"/>
+      <c r="Q43" s="31"/>
+      <c r="R43" s="32"/>
+      <c r="S43" s="32"/>
+      <c r="T43" s="32"/>
+      <c r="U43" s="33"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
@@ -2189,15 +2230,15 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
-      <c r="M44" s="30"/>
-      <c r="N44" s="30"/>
-      <c r="O44" s="30"/>
+      <c r="M44" s="21"/>
+      <c r="N44" s="21"/>
+      <c r="O44" s="21"/>
       <c r="P44" s="4"/>
-      <c r="Q44" s="25"/>
-      <c r="R44" s="26"/>
-      <c r="S44" s="26"/>
-      <c r="T44" s="26"/>
-      <c r="U44" s="27"/>
+      <c r="Q44" s="31"/>
+      <c r="R44" s="32"/>
+      <c r="S44" s="32"/>
+      <c r="T44" s="32"/>
+      <c r="U44" s="33"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
@@ -2214,15 +2255,15 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
-      <c r="M45" s="30"/>
-      <c r="N45" s="30"/>
-      <c r="O45" s="30"/>
+      <c r="M45" s="21"/>
+      <c r="N45" s="21"/>
+      <c r="O45" s="21"/>
       <c r="P45" s="4"/>
-      <c r="Q45" s="25"/>
-      <c r="R45" s="26"/>
-      <c r="S45" s="26"/>
-      <c r="T45" s="26"/>
-      <c r="U45" s="27"/>
+      <c r="Q45" s="31"/>
+      <c r="R45" s="32"/>
+      <c r="S45" s="32"/>
+      <c r="T45" s="32"/>
+      <c r="U45" s="33"/>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
@@ -2239,15 +2280,15 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
-      <c r="M46" s="30"/>
-      <c r="N46" s="30"/>
-      <c r="O46" s="30"/>
+      <c r="M46" s="21"/>
+      <c r="N46" s="21"/>
+      <c r="O46" s="21"/>
       <c r="P46" s="4"/>
-      <c r="Q46" s="25"/>
-      <c r="R46" s="26"/>
-      <c r="S46" s="26"/>
-      <c r="T46" s="26"/>
-      <c r="U46" s="27"/>
+      <c r="Q46" s="31"/>
+      <c r="R46" s="32"/>
+      <c r="S46" s="32"/>
+      <c r="T46" s="32"/>
+      <c r="U46" s="33"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
@@ -2264,15 +2305,15 @@
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
-      <c r="M47" s="30"/>
-      <c r="N47" s="30"/>
-      <c r="O47" s="30"/>
+      <c r="M47" s="21"/>
+      <c r="N47" s="21"/>
+      <c r="O47" s="21"/>
       <c r="P47" s="4"/>
-      <c r="Q47" s="25"/>
-      <c r="R47" s="26"/>
-      <c r="S47" s="26"/>
-      <c r="T47" s="26"/>
-      <c r="U47" s="27"/>
+      <c r="Q47" s="31"/>
+      <c r="R47" s="32"/>
+      <c r="S47" s="32"/>
+      <c r="T47" s="32"/>
+      <c r="U47" s="33"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
@@ -2289,15 +2330,15 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
-      <c r="M48" s="30"/>
-      <c r="N48" s="30"/>
-      <c r="O48" s="30"/>
+      <c r="M48" s="21"/>
+      <c r="N48" s="21"/>
+      <c r="O48" s="21"/>
       <c r="P48" s="4"/>
-      <c r="Q48" s="25"/>
-      <c r="R48" s="26"/>
-      <c r="S48" s="26"/>
-      <c r="T48" s="26"/>
-      <c r="U48" s="27"/>
+      <c r="Q48" s="31"/>
+      <c r="R48" s="32"/>
+      <c r="S48" s="32"/>
+      <c r="T48" s="32"/>
+      <c r="U48" s="33"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
@@ -2314,15 +2355,15 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
-      <c r="M49" s="30"/>
-      <c r="N49" s="30"/>
-      <c r="O49" s="30"/>
+      <c r="M49" s="21"/>
+      <c r="N49" s="21"/>
+      <c r="O49" s="21"/>
       <c r="P49" s="4"/>
-      <c r="Q49" s="25"/>
-      <c r="R49" s="26"/>
-      <c r="S49" s="26"/>
-      <c r="T49" s="26"/>
-      <c r="U49" s="27"/>
+      <c r="Q49" s="31"/>
+      <c r="R49" s="32"/>
+      <c r="S49" s="32"/>
+      <c r="T49" s="32"/>
+      <c r="U49" s="33"/>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
@@ -2339,15 +2380,15 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
-      <c r="M50" s="30"/>
-      <c r="N50" s="30"/>
-      <c r="O50" s="30"/>
+      <c r="M50" s="21"/>
+      <c r="N50" s="21"/>
+      <c r="O50" s="21"/>
       <c r="P50" s="4"/>
-      <c r="Q50" s="25"/>
-      <c r="R50" s="26"/>
-      <c r="S50" s="26"/>
-      <c r="T50" s="26"/>
-      <c r="U50" s="27"/>
+      <c r="Q50" s="31"/>
+      <c r="R50" s="32"/>
+      <c r="S50" s="32"/>
+      <c r="T50" s="32"/>
+      <c r="U50" s="33"/>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
@@ -2364,15 +2405,15 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
-      <c r="M51" s="30"/>
-      <c r="N51" s="30"/>
-      <c r="O51" s="30"/>
+      <c r="M51" s="21"/>
+      <c r="N51" s="21"/>
+      <c r="O51" s="21"/>
       <c r="P51" s="4"/>
-      <c r="Q51" s="25"/>
-      <c r="R51" s="26"/>
-      <c r="S51" s="26"/>
-      <c r="T51" s="26"/>
-      <c r="U51" s="27"/>
+      <c r="Q51" s="31"/>
+      <c r="R51" s="32"/>
+      <c r="S51" s="32"/>
+      <c r="T51" s="32"/>
+      <c r="U51" s="33"/>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
@@ -2389,18 +2430,18 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
-      <c r="M52" s="30"/>
-      <c r="N52" s="30"/>
-      <c r="O52" s="30"/>
+      <c r="M52" s="21"/>
+      <c r="N52" s="21"/>
+      <c r="O52" s="21"/>
       <c r="P52" s="4"/>
-      <c r="Q52" s="25"/>
-      <c r="R52" s="26"/>
-      <c r="S52" s="26"/>
-      <c r="T52" s="26"/>
-      <c r="U52" s="27"/>
+      <c r="Q52" s="31"/>
+      <c r="R52" s="32"/>
+      <c r="S52" s="32"/>
+      <c r="T52" s="32"/>
+      <c r="U52" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="52">
+  <mergeCells count="42">
     <mergeCell ref="Q48:U48"/>
     <mergeCell ref="Q49:U49"/>
     <mergeCell ref="Q50:U50"/>
@@ -2419,9 +2460,6 @@
     <mergeCell ref="Q45:U45"/>
     <mergeCell ref="Q46:U46"/>
     <mergeCell ref="Q35:U35"/>
-    <mergeCell ref="Q24:U24"/>
-    <mergeCell ref="Q25:U25"/>
-    <mergeCell ref="Q26:U26"/>
     <mergeCell ref="Q27:U27"/>
     <mergeCell ref="Q28:U28"/>
     <mergeCell ref="Q29:U29"/>
@@ -2430,18 +2468,11 @@
     <mergeCell ref="Q32:U32"/>
     <mergeCell ref="Q33:U33"/>
     <mergeCell ref="Q34:U34"/>
-    <mergeCell ref="Q23:U23"/>
     <mergeCell ref="Q12:U12"/>
     <mergeCell ref="Q13:U13"/>
     <mergeCell ref="Q14:U14"/>
     <mergeCell ref="Q15:U15"/>
     <mergeCell ref="Q16:U16"/>
-    <mergeCell ref="Q17:U17"/>
-    <mergeCell ref="Q18:U18"/>
-    <mergeCell ref="Q19:U19"/>
-    <mergeCell ref="Q20:U20"/>
-    <mergeCell ref="Q21:U21"/>
-    <mergeCell ref="Q22:U22"/>
     <mergeCell ref="Q11:U11"/>
     <mergeCell ref="E2:P2"/>
     <mergeCell ref="Q2:U2"/>

</xml_diff>

<commit_message>
Add role add messages
</commit_message>
<xml_diff>
--- a/01_Documents/Message_List_20180321.xlsx
+++ b/01_Documents/Message_List_20180321.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="52">
   <si>
     <t>#</t>
   </si>
@@ -147,7 +147,31 @@
     <t>check_moderator</t>
   </si>
   <si>
-    <t>get_content</t>
+    <t>get_content_list</t>
+  </si>
+  <si>
+    <t>Content list</t>
+  </si>
+  <si>
+    <t>approve_content</t>
+  </si>
+  <si>
+    <t>Content ID</t>
+  </si>
+  <si>
+    <t>add_role_define</t>
+  </si>
+  <si>
+    <t>Role name</t>
+  </si>
+  <si>
+    <t>add_role</t>
+  </si>
+  <si>
+    <t>Role ID</t>
+  </si>
+  <si>
+    <t>Role Code</t>
   </si>
 </sst>
 </file>
@@ -524,6 +548,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -549,15 +582,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -863,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -902,27 +926,27 @@
       <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="25" t="s">
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="27"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="30"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
@@ -953,11 +977,11 @@
       <c r="N3" s="19"/>
       <c r="O3" s="19"/>
       <c r="P3" s="10"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="30"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="33"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
@@ -998,11 +1022,11 @@
       <c r="N4" s="20"/>
       <c r="O4" s="20"/>
       <c r="P4" s="14"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="24"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="27"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
@@ -1033,11 +1057,11 @@
       <c r="N5" s="20"/>
       <c r="O5" s="20"/>
       <c r="P5" s="14"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="24"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="27"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
@@ -1066,11 +1090,11 @@
       <c r="N6" s="20"/>
       <c r="O6" s="20"/>
       <c r="P6" s="14"/>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="24"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="27"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
@@ -1101,11 +1125,11 @@
       <c r="N7" s="20"/>
       <c r="O7" s="20"/>
       <c r="P7" s="14"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="24"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="27"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
@@ -1134,11 +1158,11 @@
       <c r="N8" s="20"/>
       <c r="O8" s="20"/>
       <c r="P8" s="14"/>
-      <c r="Q8" s="22"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="24"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="26"/>
+      <c r="S8" s="26"/>
+      <c r="T8" s="26"/>
+      <c r="U8" s="27"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
@@ -1177,11 +1201,11 @@
       <c r="N9" s="20"/>
       <c r="O9" s="20"/>
       <c r="P9" s="14"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="24"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="26"/>
+      <c r="S9" s="26"/>
+      <c r="T9" s="26"/>
+      <c r="U9" s="27"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
@@ -1210,11 +1234,11 @@
       <c r="N10" s="20"/>
       <c r="O10" s="20"/>
       <c r="P10" s="14"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="24"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="26"/>
+      <c r="S10" s="26"/>
+      <c r="T10" s="26"/>
+      <c r="U10" s="27"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
@@ -1245,11 +1269,11 @@
       <c r="N11" s="20"/>
       <c r="O11" s="20"/>
       <c r="P11" s="14"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="24"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="26"/>
+      <c r="T11" s="26"/>
+      <c r="U11" s="27"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
@@ -1278,11 +1302,11 @@
       <c r="N12" s="20"/>
       <c r="O12" s="20"/>
       <c r="P12" s="14"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="24"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="26"/>
+      <c r="S12" s="26"/>
+      <c r="T12" s="26"/>
+      <c r="U12" s="27"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
@@ -1311,11 +1335,11 @@
       <c r="N13" s="20"/>
       <c r="O13" s="20"/>
       <c r="P13" s="14"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="24"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="26"/>
+      <c r="T13" s="26"/>
+      <c r="U13" s="27"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
@@ -1344,11 +1368,11 @@
       <c r="N14" s="20"/>
       <c r="O14" s="20"/>
       <c r="P14" s="14"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="23"/>
-      <c r="U14" s="24"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="26"/>
+      <c r="S14" s="26"/>
+      <c r="T14" s="26"/>
+      <c r="U14" s="27"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
@@ -1379,11 +1403,11 @@
       <c r="N15" s="20"/>
       <c r="O15" s="20"/>
       <c r="P15" s="14"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="24"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="26"/>
+      <c r="S15" s="26"/>
+      <c r="T15" s="26"/>
+      <c r="U15" s="27"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
@@ -1412,11 +1436,11 @@
       <c r="N16" s="20"/>
       <c r="O16" s="20"/>
       <c r="P16" s="14"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="24"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="26"/>
+      <c r="S16" s="26"/>
+      <c r="T16" s="26"/>
+      <c r="U16" s="27"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
@@ -1791,7 +1815,9 @@
       <c r="D27" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="13"/>
+      <c r="E27" s="13" t="s">
+        <v>28</v>
+      </c>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
@@ -1803,11 +1829,11 @@
       <c r="N27" s="20"/>
       <c r="O27" s="20"/>
       <c r="P27" s="14"/>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="23"/>
-      <c r="S27" s="23"/>
-      <c r="T27" s="23"/>
-      <c r="U27" s="24"/>
+      <c r="Q27" s="25"/>
+      <c r="R27" s="26"/>
+      <c r="S27" s="26"/>
+      <c r="T27" s="26"/>
+      <c r="U27" s="27"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
@@ -1822,8 +1848,12 @@
       <c r="D28" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="15"/>
+      <c r="E28" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>44</v>
+      </c>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
@@ -1834,21 +1864,31 @@
       <c r="N28" s="20"/>
       <c r="O28" s="20"/>
       <c r="P28" s="14"/>
-      <c r="Q28" s="22"/>
-      <c r="R28" s="23"/>
-      <c r="S28" s="23"/>
-      <c r="T28" s="23"/>
-      <c r="U28" s="24"/>
+      <c r="Q28" s="25"/>
+      <c r="R28" s="26"/>
+      <c r="S28" s="26"/>
+      <c r="T28" s="26"/>
+      <c r="U28" s="27"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>27</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="15"/>
+      <c r="B29" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>46</v>
+      </c>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
@@ -1859,20 +1899,28 @@
       <c r="N29" s="20"/>
       <c r="O29" s="20"/>
       <c r="P29" s="14"/>
-      <c r="Q29" s="22"/>
-      <c r="R29" s="23"/>
-      <c r="S29" s="23"/>
-      <c r="T29" s="23"/>
-      <c r="U29" s="24"/>
+      <c r="Q29" s="25"/>
+      <c r="R29" s="26"/>
+      <c r="S29" s="26"/>
+      <c r="T29" s="26"/>
+      <c r="U29" s="27"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>28</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="13"/>
+      <c r="B30" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>15</v>
+      </c>
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
@@ -1884,21 +1932,31 @@
       <c r="N30" s="20"/>
       <c r="O30" s="20"/>
       <c r="P30" s="14"/>
-      <c r="Q30" s="22"/>
-      <c r="R30" s="23"/>
-      <c r="S30" s="23"/>
-      <c r="T30" s="23"/>
-      <c r="U30" s="24"/>
+      <c r="Q30" s="25"/>
+      <c r="R30" s="26"/>
+      <c r="S30" s="26"/>
+      <c r="T30" s="26"/>
+      <c r="U30" s="27"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>29</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="15"/>
+      <c r="B31" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>48</v>
+      </c>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
@@ -1909,20 +1967,28 @@
       <c r="N31" s="20"/>
       <c r="O31" s="20"/>
       <c r="P31" s="14"/>
-      <c r="Q31" s="22"/>
-      <c r="R31" s="23"/>
-      <c r="S31" s="23"/>
-      <c r="T31" s="23"/>
-      <c r="U31" s="24"/>
+      <c r="Q31" s="25"/>
+      <c r="R31" s="26"/>
+      <c r="S31" s="26"/>
+      <c r="T31" s="26"/>
+      <c r="U31" s="27"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>30</v>
       </c>
-      <c r="B32" s="12"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="13"/>
+      <c r="B32" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>15</v>
+      </c>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
@@ -1934,23 +2000,37 @@
       <c r="N32" s="20"/>
       <c r="O32" s="20"/>
       <c r="P32" s="14"/>
-      <c r="Q32" s="22"/>
-      <c r="R32" s="23"/>
-      <c r="S32" s="23"/>
-      <c r="T32" s="23"/>
-      <c r="U32" s="24"/>
+      <c r="Q32" s="25"/>
+      <c r="R32" s="26"/>
+      <c r="S32" s="26"/>
+      <c r="T32" s="26"/>
+      <c r="U32" s="27"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>31</v>
       </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
+      <c r="B33" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H33" s="15" t="s">
+        <v>51</v>
+      </c>
       <c r="I33" s="15"/>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
@@ -1959,20 +2039,28 @@
       <c r="N33" s="20"/>
       <c r="O33" s="20"/>
       <c r="P33" s="14"/>
-      <c r="Q33" s="22"/>
-      <c r="R33" s="23"/>
-      <c r="S33" s="23"/>
-      <c r="T33" s="23"/>
-      <c r="U33" s="24"/>
+      <c r="Q33" s="25"/>
+      <c r="R33" s="26"/>
+      <c r="S33" s="26"/>
+      <c r="T33" s="26"/>
+      <c r="U33" s="27"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>32</v>
       </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="13"/>
+      <c r="B34" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>15</v>
+      </c>
       <c r="F34" s="15"/>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
@@ -1984,11 +2072,11 @@
       <c r="N34" s="20"/>
       <c r="O34" s="20"/>
       <c r="P34" s="14"/>
-      <c r="Q34" s="22"/>
-      <c r="R34" s="23"/>
-      <c r="S34" s="23"/>
-      <c r="T34" s="23"/>
-      <c r="U34" s="24"/>
+      <c r="Q34" s="25"/>
+      <c r="R34" s="26"/>
+      <c r="S34" s="26"/>
+      <c r="T34" s="26"/>
+      <c r="U34" s="27"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
@@ -2009,11 +2097,11 @@
       <c r="N35" s="20"/>
       <c r="O35" s="20"/>
       <c r="P35" s="14"/>
-      <c r="Q35" s="22"/>
-      <c r="R35" s="23"/>
-      <c r="S35" s="23"/>
-      <c r="T35" s="23"/>
-      <c r="U35" s="24"/>
+      <c r="Q35" s="25"/>
+      <c r="R35" s="26"/>
+      <c r="S35" s="26"/>
+      <c r="T35" s="26"/>
+      <c r="U35" s="27"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A36" s="12">
@@ -2034,11 +2122,11 @@
       <c r="N36" s="20"/>
       <c r="O36" s="20"/>
       <c r="P36" s="14"/>
-      <c r="Q36" s="22"/>
-      <c r="R36" s="23"/>
-      <c r="S36" s="23"/>
-      <c r="T36" s="23"/>
-      <c r="U36" s="24"/>
+      <c r="Q36" s="25"/>
+      <c r="R36" s="26"/>
+      <c r="S36" s="26"/>
+      <c r="T36" s="26"/>
+      <c r="U36" s="27"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A37" s="12">
@@ -2059,11 +2147,11 @@
       <c r="N37" s="20"/>
       <c r="O37" s="20"/>
       <c r="P37" s="14"/>
-      <c r="Q37" s="22"/>
-      <c r="R37" s="23"/>
-      <c r="S37" s="23"/>
-      <c r="T37" s="23"/>
-      <c r="U37" s="24"/>
+      <c r="Q37" s="25"/>
+      <c r="R37" s="26"/>
+      <c r="S37" s="26"/>
+      <c r="T37" s="26"/>
+      <c r="U37" s="27"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A38" s="12">
@@ -2084,11 +2172,11 @@
       <c r="N38" s="20"/>
       <c r="O38" s="20"/>
       <c r="P38" s="14"/>
-      <c r="Q38" s="22"/>
-      <c r="R38" s="23"/>
-      <c r="S38" s="23"/>
-      <c r="T38" s="23"/>
-      <c r="U38" s="24"/>
+      <c r="Q38" s="25"/>
+      <c r="R38" s="26"/>
+      <c r="S38" s="26"/>
+      <c r="T38" s="26"/>
+      <c r="U38" s="27"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A39" s="12">
@@ -2109,11 +2197,11 @@
       <c r="N39" s="20"/>
       <c r="O39" s="20"/>
       <c r="P39" s="14"/>
-      <c r="Q39" s="22"/>
-      <c r="R39" s="23"/>
-      <c r="S39" s="23"/>
-      <c r="T39" s="23"/>
-      <c r="U39" s="24"/>
+      <c r="Q39" s="25"/>
+      <c r="R39" s="26"/>
+      <c r="S39" s="26"/>
+      <c r="T39" s="26"/>
+      <c r="U39" s="27"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
@@ -2134,11 +2222,11 @@
       <c r="N40" s="21"/>
       <c r="O40" s="21"/>
       <c r="P40" s="4"/>
-      <c r="Q40" s="31"/>
-      <c r="R40" s="32"/>
-      <c r="S40" s="32"/>
-      <c r="T40" s="32"/>
-      <c r="U40" s="33"/>
+      <c r="Q40" s="22"/>
+      <c r="R40" s="23"/>
+      <c r="S40" s="23"/>
+      <c r="T40" s="23"/>
+      <c r="U40" s="24"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
@@ -2159,11 +2247,11 @@
       <c r="N41" s="21"/>
       <c r="O41" s="21"/>
       <c r="P41" s="4"/>
-      <c r="Q41" s="31"/>
-      <c r="R41" s="32"/>
-      <c r="S41" s="32"/>
-      <c r="T41" s="32"/>
-      <c r="U41" s="33"/>
+      <c r="Q41" s="22"/>
+      <c r="R41" s="23"/>
+      <c r="S41" s="23"/>
+      <c r="T41" s="23"/>
+      <c r="U41" s="24"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
@@ -2184,11 +2272,11 @@
       <c r="N42" s="21"/>
       <c r="O42" s="21"/>
       <c r="P42" s="4"/>
-      <c r="Q42" s="31"/>
-      <c r="R42" s="32"/>
-      <c r="S42" s="32"/>
-      <c r="T42" s="32"/>
-      <c r="U42" s="33"/>
+      <c r="Q42" s="22"/>
+      <c r="R42" s="23"/>
+      <c r="S42" s="23"/>
+      <c r="T42" s="23"/>
+      <c r="U42" s="24"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
@@ -2209,11 +2297,11 @@
       <c r="N43" s="21"/>
       <c r="O43" s="21"/>
       <c r="P43" s="4"/>
-      <c r="Q43" s="31"/>
-      <c r="R43" s="32"/>
-      <c r="S43" s="32"/>
-      <c r="T43" s="32"/>
-      <c r="U43" s="33"/>
+      <c r="Q43" s="22"/>
+      <c r="R43" s="23"/>
+      <c r="S43" s="23"/>
+      <c r="T43" s="23"/>
+      <c r="U43" s="24"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
@@ -2234,11 +2322,11 @@
       <c r="N44" s="21"/>
       <c r="O44" s="21"/>
       <c r="P44" s="4"/>
-      <c r="Q44" s="31"/>
-      <c r="R44" s="32"/>
-      <c r="S44" s="32"/>
-      <c r="T44" s="32"/>
-      <c r="U44" s="33"/>
+      <c r="Q44" s="22"/>
+      <c r="R44" s="23"/>
+      <c r="S44" s="23"/>
+      <c r="T44" s="23"/>
+      <c r="U44" s="24"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
@@ -2259,11 +2347,11 @@
       <c r="N45" s="21"/>
       <c r="O45" s="21"/>
       <c r="P45" s="4"/>
-      <c r="Q45" s="31"/>
-      <c r="R45" s="32"/>
-      <c r="S45" s="32"/>
-      <c r="T45" s="32"/>
-      <c r="U45" s="33"/>
+      <c r="Q45" s="22"/>
+      <c r="R45" s="23"/>
+      <c r="S45" s="23"/>
+      <c r="T45" s="23"/>
+      <c r="U45" s="24"/>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
@@ -2284,11 +2372,11 @@
       <c r="N46" s="21"/>
       <c r="O46" s="21"/>
       <c r="P46" s="4"/>
-      <c r="Q46" s="31"/>
-      <c r="R46" s="32"/>
-      <c r="S46" s="32"/>
-      <c r="T46" s="32"/>
-      <c r="U46" s="33"/>
+      <c r="Q46" s="22"/>
+      <c r="R46" s="23"/>
+      <c r="S46" s="23"/>
+      <c r="T46" s="23"/>
+      <c r="U46" s="24"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
@@ -2309,11 +2397,11 @@
       <c r="N47" s="21"/>
       <c r="O47" s="21"/>
       <c r="P47" s="4"/>
-      <c r="Q47" s="31"/>
-      <c r="R47" s="32"/>
-      <c r="S47" s="32"/>
-      <c r="T47" s="32"/>
-      <c r="U47" s="33"/>
+      <c r="Q47" s="22"/>
+      <c r="R47" s="23"/>
+      <c r="S47" s="23"/>
+      <c r="T47" s="23"/>
+      <c r="U47" s="24"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
@@ -2334,11 +2422,11 @@
       <c r="N48" s="21"/>
       <c r="O48" s="21"/>
       <c r="P48" s="4"/>
-      <c r="Q48" s="31"/>
-      <c r="R48" s="32"/>
-      <c r="S48" s="32"/>
-      <c r="T48" s="32"/>
-      <c r="U48" s="33"/>
+      <c r="Q48" s="22"/>
+      <c r="R48" s="23"/>
+      <c r="S48" s="23"/>
+      <c r="T48" s="23"/>
+      <c r="U48" s="24"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
@@ -2359,11 +2447,11 @@
       <c r="N49" s="21"/>
       <c r="O49" s="21"/>
       <c r="P49" s="4"/>
-      <c r="Q49" s="31"/>
-      <c r="R49" s="32"/>
-      <c r="S49" s="32"/>
-      <c r="T49" s="32"/>
-      <c r="U49" s="33"/>
+      <c r="Q49" s="22"/>
+      <c r="R49" s="23"/>
+      <c r="S49" s="23"/>
+      <c r="T49" s="23"/>
+      <c r="U49" s="24"/>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
@@ -2384,11 +2472,11 @@
       <c r="N50" s="21"/>
       <c r="O50" s="21"/>
       <c r="P50" s="4"/>
-      <c r="Q50" s="31"/>
-      <c r="R50" s="32"/>
-      <c r="S50" s="32"/>
-      <c r="T50" s="32"/>
-      <c r="U50" s="33"/>
+      <c r="Q50" s="22"/>
+      <c r="R50" s="23"/>
+      <c r="S50" s="23"/>
+      <c r="T50" s="23"/>
+      <c r="U50" s="24"/>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
@@ -2409,11 +2497,11 @@
       <c r="N51" s="21"/>
       <c r="O51" s="21"/>
       <c r="P51" s="4"/>
-      <c r="Q51" s="31"/>
-      <c r="R51" s="32"/>
-      <c r="S51" s="32"/>
-      <c r="T51" s="32"/>
-      <c r="U51" s="33"/>
+      <c r="Q51" s="22"/>
+      <c r="R51" s="23"/>
+      <c r="S51" s="23"/>
+      <c r="T51" s="23"/>
+      <c r="U51" s="24"/>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
@@ -2434,19 +2522,39 @@
       <c r="N52" s="21"/>
       <c r="O52" s="21"/>
       <c r="P52" s="4"/>
-      <c r="Q52" s="31"/>
-      <c r="R52" s="32"/>
-      <c r="S52" s="32"/>
-      <c r="T52" s="32"/>
-      <c r="U52" s="33"/>
+      <c r="Q52" s="22"/>
+      <c r="R52" s="23"/>
+      <c r="S52" s="23"/>
+      <c r="T52" s="23"/>
+      <c r="U52" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="Q48:U48"/>
-    <mergeCell ref="Q49:U49"/>
-    <mergeCell ref="Q50:U50"/>
-    <mergeCell ref="Q51:U51"/>
-    <mergeCell ref="Q52:U52"/>
+    <mergeCell ref="Q11:U11"/>
+    <mergeCell ref="E2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="Q6:U6"/>
+    <mergeCell ref="Q7:U7"/>
+    <mergeCell ref="Q8:U8"/>
+    <mergeCell ref="Q9:U9"/>
+    <mergeCell ref="Q10:U10"/>
+    <mergeCell ref="Q12:U12"/>
+    <mergeCell ref="Q13:U13"/>
+    <mergeCell ref="Q14:U14"/>
+    <mergeCell ref="Q15:U15"/>
+    <mergeCell ref="Q16:U16"/>
+    <mergeCell ref="Q35:U35"/>
+    <mergeCell ref="Q27:U27"/>
+    <mergeCell ref="Q28:U28"/>
+    <mergeCell ref="Q29:U29"/>
+    <mergeCell ref="Q30:U30"/>
+    <mergeCell ref="Q31:U31"/>
+    <mergeCell ref="Q32:U32"/>
+    <mergeCell ref="Q33:U33"/>
+    <mergeCell ref="Q34:U34"/>
     <mergeCell ref="Q47:U47"/>
     <mergeCell ref="Q36:U36"/>
     <mergeCell ref="Q38:U38"/>
@@ -2459,31 +2567,11 @@
     <mergeCell ref="Q44:U44"/>
     <mergeCell ref="Q45:U45"/>
     <mergeCell ref="Q46:U46"/>
-    <mergeCell ref="Q35:U35"/>
-    <mergeCell ref="Q27:U27"/>
-    <mergeCell ref="Q28:U28"/>
-    <mergeCell ref="Q29:U29"/>
-    <mergeCell ref="Q30:U30"/>
-    <mergeCell ref="Q31:U31"/>
-    <mergeCell ref="Q32:U32"/>
-    <mergeCell ref="Q33:U33"/>
-    <mergeCell ref="Q34:U34"/>
-    <mergeCell ref="Q12:U12"/>
-    <mergeCell ref="Q13:U13"/>
-    <mergeCell ref="Q14:U14"/>
-    <mergeCell ref="Q15:U15"/>
-    <mergeCell ref="Q16:U16"/>
-    <mergeCell ref="Q11:U11"/>
-    <mergeCell ref="E2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="Q4:U4"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="Q6:U6"/>
-    <mergeCell ref="Q7:U7"/>
-    <mergeCell ref="Q8:U8"/>
-    <mergeCell ref="Q9:U9"/>
-    <mergeCell ref="Q10:U10"/>
+    <mergeCell ref="Q48:U48"/>
+    <mergeCell ref="Q49:U49"/>
+    <mergeCell ref="Q50:U50"/>
+    <mergeCell ref="Q51:U51"/>
+    <mergeCell ref="Q52:U52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add source code which has MIT license, worked
</commit_message>
<xml_diff>
--- a/01_Documents/Message_List_20180321.xlsx
+++ b/01_Documents/Message_List_20180321.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="59">
   <si>
     <t>#</t>
   </si>
@@ -172,6 +172,27 @@
   </si>
   <si>
     <t>Role Code</t>
+  </si>
+  <si>
+    <t>add_transaction</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>get_content_list_by_user</t>
+  </si>
+  <si>
+    <t>get_content_list_owner</t>
+  </si>
+  <si>
+    <t>get_content</t>
+  </si>
+  <si>
+    <t>Session Code (?)</t>
   </si>
 </sst>
 </file>
@@ -548,15 +569,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -582,6 +594,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -887,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -899,7 +920,7 @@
     <col min="5" max="5" width="18.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.54296875" bestFit="1" customWidth="1"/>
@@ -926,27 +947,27 @@
       <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="28" t="s">
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="30"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="27"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
@@ -977,11 +998,11 @@
       <c r="N3" s="19"/>
       <c r="O3" s="19"/>
       <c r="P3" s="10"/>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
-      <c r="T3" s="32"/>
-      <c r="U3" s="33"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="30"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
@@ -1022,11 +1043,11 @@
       <c r="N4" s="20"/>
       <c r="O4" s="20"/>
       <c r="P4" s="14"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
-      <c r="U4" s="27"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="24"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
@@ -1057,11 +1078,11 @@
       <c r="N5" s="20"/>
       <c r="O5" s="20"/>
       <c r="P5" s="14"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
-      <c r="U5" s="27"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="24"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
@@ -1090,11 +1111,11 @@
       <c r="N6" s="20"/>
       <c r="O6" s="20"/>
       <c r="P6" s="14"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="26"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="26"/>
-      <c r="U6" s="27"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="24"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
@@ -1125,11 +1146,11 @@
       <c r="N7" s="20"/>
       <c r="O7" s="20"/>
       <c r="P7" s="14"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
-      <c r="U7" s="27"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="24"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
@@ -1158,11 +1179,11 @@
       <c r="N8" s="20"/>
       <c r="O8" s="20"/>
       <c r="P8" s="14"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="26"/>
-      <c r="S8" s="26"/>
-      <c r="T8" s="26"/>
-      <c r="U8" s="27"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="24"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
@@ -1201,11 +1222,11 @@
       <c r="N9" s="20"/>
       <c r="O9" s="20"/>
       <c r="P9" s="14"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="26"/>
-      <c r="S9" s="26"/>
-      <c r="T9" s="26"/>
-      <c r="U9" s="27"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="24"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
@@ -1234,11 +1255,11 @@
       <c r="N10" s="20"/>
       <c r="O10" s="20"/>
       <c r="P10" s="14"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="26"/>
-      <c r="S10" s="26"/>
-      <c r="T10" s="26"/>
-      <c r="U10" s="27"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="24"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
@@ -1269,11 +1290,11 @@
       <c r="N11" s="20"/>
       <c r="O11" s="20"/>
       <c r="P11" s="14"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="26"/>
-      <c r="S11" s="26"/>
-      <c r="T11" s="26"/>
-      <c r="U11" s="27"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="24"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
@@ -1302,11 +1323,11 @@
       <c r="N12" s="20"/>
       <c r="O12" s="20"/>
       <c r="P12" s="14"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="26"/>
-      <c r="S12" s="26"/>
-      <c r="T12" s="26"/>
-      <c r="U12" s="27"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="24"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
@@ -1335,11 +1356,11 @@
       <c r="N13" s="20"/>
       <c r="O13" s="20"/>
       <c r="P13" s="14"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="26"/>
-      <c r="S13" s="26"/>
-      <c r="T13" s="26"/>
-      <c r="U13" s="27"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
+      <c r="U13" s="24"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
@@ -1368,11 +1389,11 @@
       <c r="N14" s="20"/>
       <c r="O14" s="20"/>
       <c r="P14" s="14"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="26"/>
-      <c r="S14" s="26"/>
-      <c r="T14" s="26"/>
-      <c r="U14" s="27"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23"/>
+      <c r="T14" s="23"/>
+      <c r="U14" s="24"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
@@ -1403,11 +1424,11 @@
       <c r="N15" s="20"/>
       <c r="O15" s="20"/>
       <c r="P15" s="14"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="26"/>
-      <c r="S15" s="26"/>
-      <c r="T15" s="26"/>
-      <c r="U15" s="27"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="24"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
@@ -1436,11 +1457,11 @@
       <c r="N16" s="20"/>
       <c r="O16" s="20"/>
       <c r="P16" s="14"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="26"/>
-      <c r="S16" s="26"/>
-      <c r="T16" s="26"/>
-      <c r="U16" s="27"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="24"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
@@ -1829,11 +1850,11 @@
       <c r="N27" s="20"/>
       <c r="O27" s="20"/>
       <c r="P27" s="14"/>
-      <c r="Q27" s="25"/>
-      <c r="R27" s="26"/>
-      <c r="S27" s="26"/>
-      <c r="T27" s="26"/>
-      <c r="U27" s="27"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="23"/>
+      <c r="S27" s="23"/>
+      <c r="T27" s="23"/>
+      <c r="U27" s="24"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
@@ -1864,11 +1885,11 @@
       <c r="N28" s="20"/>
       <c r="O28" s="20"/>
       <c r="P28" s="14"/>
-      <c r="Q28" s="25"/>
-      <c r="R28" s="26"/>
-      <c r="S28" s="26"/>
-      <c r="T28" s="26"/>
-      <c r="U28" s="27"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="23"/>
+      <c r="S28" s="23"/>
+      <c r="T28" s="23"/>
+      <c r="U28" s="24"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
@@ -1899,11 +1920,11 @@
       <c r="N29" s="20"/>
       <c r="O29" s="20"/>
       <c r="P29" s="14"/>
-      <c r="Q29" s="25"/>
-      <c r="R29" s="26"/>
-      <c r="S29" s="26"/>
-      <c r="T29" s="26"/>
-      <c r="U29" s="27"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
+      <c r="T29" s="23"/>
+      <c r="U29" s="24"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
@@ -1932,11 +1953,11 @@
       <c r="N30" s="20"/>
       <c r="O30" s="20"/>
       <c r="P30" s="14"/>
-      <c r="Q30" s="25"/>
-      <c r="R30" s="26"/>
-      <c r="S30" s="26"/>
-      <c r="T30" s="26"/>
-      <c r="U30" s="27"/>
+      <c r="Q30" s="22"/>
+      <c r="R30" s="23"/>
+      <c r="S30" s="23"/>
+      <c r="T30" s="23"/>
+      <c r="U30" s="24"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
@@ -1967,11 +1988,11 @@
       <c r="N31" s="20"/>
       <c r="O31" s="20"/>
       <c r="P31" s="14"/>
-      <c r="Q31" s="25"/>
-      <c r="R31" s="26"/>
-      <c r="S31" s="26"/>
-      <c r="T31" s="26"/>
-      <c r="U31" s="27"/>
+      <c r="Q31" s="22"/>
+      <c r="R31" s="23"/>
+      <c r="S31" s="23"/>
+      <c r="T31" s="23"/>
+      <c r="U31" s="24"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
@@ -2000,11 +2021,11 @@
       <c r="N32" s="20"/>
       <c r="O32" s="20"/>
       <c r="P32" s="14"/>
-      <c r="Q32" s="25"/>
-      <c r="R32" s="26"/>
-      <c r="S32" s="26"/>
-      <c r="T32" s="26"/>
-      <c r="U32" s="27"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="23"/>
+      <c r="S32" s="23"/>
+      <c r="T32" s="23"/>
+      <c r="U32" s="24"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
@@ -2039,11 +2060,11 @@
       <c r="N33" s="20"/>
       <c r="O33" s="20"/>
       <c r="P33" s="14"/>
-      <c r="Q33" s="25"/>
-      <c r="R33" s="26"/>
-      <c r="S33" s="26"/>
-      <c r="T33" s="26"/>
-      <c r="U33" s="27"/>
+      <c r="Q33" s="22"/>
+      <c r="R33" s="23"/>
+      <c r="S33" s="23"/>
+      <c r="T33" s="23"/>
+      <c r="U33" s="24"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
@@ -2072,23 +2093,37 @@
       <c r="N34" s="20"/>
       <c r="O34" s="20"/>
       <c r="P34" s="14"/>
-      <c r="Q34" s="25"/>
-      <c r="R34" s="26"/>
-      <c r="S34" s="26"/>
-      <c r="T34" s="26"/>
-      <c r="U34" s="27"/>
+      <c r="Q34" s="22"/>
+      <c r="R34" s="23"/>
+      <c r="S34" s="23"/>
+      <c r="T34" s="23"/>
+      <c r="U34" s="24"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>33</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
+      <c r="B35" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H35" s="15" t="s">
+        <v>54</v>
+      </c>
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
@@ -2097,20 +2132,28 @@
       <c r="N35" s="20"/>
       <c r="O35" s="20"/>
       <c r="P35" s="14"/>
-      <c r="Q35" s="25"/>
-      <c r="R35" s="26"/>
-      <c r="S35" s="26"/>
-      <c r="T35" s="26"/>
-      <c r="U35" s="27"/>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="23"/>
+      <c r="S35" s="23"/>
+      <c r="T35" s="23"/>
+      <c r="U35" s="24"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A36" s="12">
         <v>34</v>
       </c>
-      <c r="B36" s="12"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="13"/>
+      <c r="B36" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>15</v>
+      </c>
       <c r="F36" s="15"/>
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
@@ -2122,20 +2165,28 @@
       <c r="N36" s="20"/>
       <c r="O36" s="20"/>
       <c r="P36" s="14"/>
-      <c r="Q36" s="25"/>
-      <c r="R36" s="26"/>
-      <c r="S36" s="26"/>
-      <c r="T36" s="26"/>
-      <c r="U36" s="27"/>
+      <c r="Q36" s="22"/>
+      <c r="R36" s="23"/>
+      <c r="S36" s="23"/>
+      <c r="T36" s="23"/>
+      <c r="U36" s="24"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A37" s="12">
         <v>35</v>
       </c>
-      <c r="B37" s="12"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="13"/>
+      <c r="B37" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
       <c r="H37" s="15"/>
@@ -2147,21 +2198,31 @@
       <c r="N37" s="20"/>
       <c r="O37" s="20"/>
       <c r="P37" s="14"/>
-      <c r="Q37" s="25"/>
-      <c r="R37" s="26"/>
-      <c r="S37" s="26"/>
-      <c r="T37" s="26"/>
-      <c r="U37" s="27"/>
+      <c r="Q37" s="22"/>
+      <c r="R37" s="23"/>
+      <c r="S37" s="23"/>
+      <c r="T37" s="23"/>
+      <c r="U37" s="24"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A38" s="12">
         <v>36</v>
       </c>
-      <c r="B38" s="12"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="15"/>
+      <c r="B38" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>44</v>
+      </c>
       <c r="G38" s="15"/>
       <c r="H38" s="15"/>
       <c r="I38" s="15"/>
@@ -2172,20 +2233,28 @@
       <c r="N38" s="20"/>
       <c r="O38" s="20"/>
       <c r="P38" s="14"/>
-      <c r="Q38" s="25"/>
-      <c r="R38" s="26"/>
-      <c r="S38" s="26"/>
-      <c r="T38" s="26"/>
-      <c r="U38" s="27"/>
+      <c r="Q38" s="22"/>
+      <c r="R38" s="23"/>
+      <c r="S38" s="23"/>
+      <c r="T38" s="23"/>
+      <c r="U38" s="24"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A39" s="12">
         <v>37</v>
       </c>
-      <c r="B39" s="12"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="13"/>
+      <c r="B39" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="F39" s="15"/>
       <c r="G39" s="15"/>
       <c r="H39" s="15"/>
@@ -2197,21 +2266,31 @@
       <c r="N39" s="20"/>
       <c r="O39" s="20"/>
       <c r="P39" s="14"/>
-      <c r="Q39" s="25"/>
-      <c r="R39" s="26"/>
-      <c r="S39" s="26"/>
-      <c r="T39" s="26"/>
-      <c r="U39" s="27"/>
+      <c r="Q39" s="22"/>
+      <c r="R39" s="23"/>
+      <c r="S39" s="23"/>
+      <c r="T39" s="23"/>
+      <c r="U39" s="24"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="1"/>
+      <c r="B40" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -2222,21 +2301,31 @@
       <c r="N40" s="21"/>
       <c r="O40" s="21"/>
       <c r="P40" s="4"/>
-      <c r="Q40" s="22"/>
-      <c r="R40" s="23"/>
-      <c r="S40" s="23"/>
-      <c r="T40" s="23"/>
-      <c r="U40" s="24"/>
+      <c r="Q40" s="31"/>
+      <c r="R40" s="32"/>
+      <c r="S40" s="32"/>
+      <c r="T40" s="32"/>
+      <c r="U40" s="33"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="1"/>
+      <c r="B41" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -2247,36 +2336,66 @@
       <c r="N41" s="21"/>
       <c r="O41" s="21"/>
       <c r="P41" s="4"/>
-      <c r="Q41" s="22"/>
-      <c r="R41" s="23"/>
-      <c r="S41" s="23"/>
-      <c r="T41" s="23"/>
-      <c r="U41" s="24"/>
+      <c r="Q41" s="31"/>
+      <c r="R41" s="32"/>
+      <c r="S41" s="32"/>
+      <c r="T41" s="32"/>
+      <c r="U41" s="33"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="21"/>
-      <c r="N42" s="21"/>
-      <c r="O42" s="21"/>
-      <c r="P42" s="4"/>
-      <c r="Q42" s="22"/>
-      <c r="R42" s="23"/>
-      <c r="S42" s="23"/>
-      <c r="T42" s="23"/>
-      <c r="U42" s="24"/>
+      <c r="B42" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G42" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I42" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J42" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K42" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L42" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="M42" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="N42" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="O42" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="P42" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q42" s="31"/>
+      <c r="R42" s="32"/>
+      <c r="S42" s="32"/>
+      <c r="T42" s="32"/>
+      <c r="U42" s="33"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
@@ -2297,11 +2416,11 @@
       <c r="N43" s="21"/>
       <c r="O43" s="21"/>
       <c r="P43" s="4"/>
-      <c r="Q43" s="22"/>
-      <c r="R43" s="23"/>
-      <c r="S43" s="23"/>
-      <c r="T43" s="23"/>
-      <c r="U43" s="24"/>
+      <c r="Q43" s="31"/>
+      <c r="R43" s="32"/>
+      <c r="S43" s="32"/>
+      <c r="T43" s="32"/>
+      <c r="U43" s="33"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
@@ -2322,11 +2441,11 @@
       <c r="N44" s="21"/>
       <c r="O44" s="21"/>
       <c r="P44" s="4"/>
-      <c r="Q44" s="22"/>
-      <c r="R44" s="23"/>
-      <c r="S44" s="23"/>
-      <c r="T44" s="23"/>
-      <c r="U44" s="24"/>
+      <c r="Q44" s="31"/>
+      <c r="R44" s="32"/>
+      <c r="S44" s="32"/>
+      <c r="T44" s="32"/>
+      <c r="U44" s="33"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
@@ -2347,11 +2466,11 @@
       <c r="N45" s="21"/>
       <c r="O45" s="21"/>
       <c r="P45" s="4"/>
-      <c r="Q45" s="22"/>
-      <c r="R45" s="23"/>
-      <c r="S45" s="23"/>
-      <c r="T45" s="23"/>
-      <c r="U45" s="24"/>
+      <c r="Q45" s="31"/>
+      <c r="R45" s="32"/>
+      <c r="S45" s="32"/>
+      <c r="T45" s="32"/>
+      <c r="U45" s="33"/>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
@@ -2372,11 +2491,11 @@
       <c r="N46" s="21"/>
       <c r="O46" s="21"/>
       <c r="P46" s="4"/>
-      <c r="Q46" s="22"/>
-      <c r="R46" s="23"/>
-      <c r="S46" s="23"/>
-      <c r="T46" s="23"/>
-      <c r="U46" s="24"/>
+      <c r="Q46" s="31"/>
+      <c r="R46" s="32"/>
+      <c r="S46" s="32"/>
+      <c r="T46" s="32"/>
+      <c r="U46" s="33"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
@@ -2397,11 +2516,11 @@
       <c r="N47" s="21"/>
       <c r="O47" s="21"/>
       <c r="P47" s="4"/>
-      <c r="Q47" s="22"/>
-      <c r="R47" s="23"/>
-      <c r="S47" s="23"/>
-      <c r="T47" s="23"/>
-      <c r="U47" s="24"/>
+      <c r="Q47" s="31"/>
+      <c r="R47" s="32"/>
+      <c r="S47" s="32"/>
+      <c r="T47" s="32"/>
+      <c r="U47" s="33"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
@@ -2422,11 +2541,11 @@
       <c r="N48" s="21"/>
       <c r="O48" s="21"/>
       <c r="P48" s="4"/>
-      <c r="Q48" s="22"/>
-      <c r="R48" s="23"/>
-      <c r="S48" s="23"/>
-      <c r="T48" s="23"/>
-      <c r="U48" s="24"/>
+      <c r="Q48" s="31"/>
+      <c r="R48" s="32"/>
+      <c r="S48" s="32"/>
+      <c r="T48" s="32"/>
+      <c r="U48" s="33"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
@@ -2447,11 +2566,11 @@
       <c r="N49" s="21"/>
       <c r="O49" s="21"/>
       <c r="P49" s="4"/>
-      <c r="Q49" s="22"/>
-      <c r="R49" s="23"/>
-      <c r="S49" s="23"/>
-      <c r="T49" s="23"/>
-      <c r="U49" s="24"/>
+      <c r="Q49" s="31"/>
+      <c r="R49" s="32"/>
+      <c r="S49" s="32"/>
+      <c r="T49" s="32"/>
+      <c r="U49" s="33"/>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
@@ -2472,11 +2591,11 @@
       <c r="N50" s="21"/>
       <c r="O50" s="21"/>
       <c r="P50" s="4"/>
-      <c r="Q50" s="22"/>
-      <c r="R50" s="23"/>
-      <c r="S50" s="23"/>
-      <c r="T50" s="23"/>
-      <c r="U50" s="24"/>
+      <c r="Q50" s="31"/>
+      <c r="R50" s="32"/>
+      <c r="S50" s="32"/>
+      <c r="T50" s="32"/>
+      <c r="U50" s="33"/>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
@@ -2497,11 +2616,11 @@
       <c r="N51" s="21"/>
       <c r="O51" s="21"/>
       <c r="P51" s="4"/>
-      <c r="Q51" s="22"/>
-      <c r="R51" s="23"/>
-      <c r="S51" s="23"/>
-      <c r="T51" s="23"/>
-      <c r="U51" s="24"/>
+      <c r="Q51" s="31"/>
+      <c r="R51" s="32"/>
+      <c r="S51" s="32"/>
+      <c r="T51" s="32"/>
+      <c r="U51" s="33"/>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
@@ -2522,39 +2641,19 @@
       <c r="N52" s="21"/>
       <c r="O52" s="21"/>
       <c r="P52" s="4"/>
-      <c r="Q52" s="22"/>
-      <c r="R52" s="23"/>
-      <c r="S52" s="23"/>
-      <c r="T52" s="23"/>
-      <c r="U52" s="24"/>
+      <c r="Q52" s="31"/>
+      <c r="R52" s="32"/>
+      <c r="S52" s="32"/>
+      <c r="T52" s="32"/>
+      <c r="U52" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="Q11:U11"/>
-    <mergeCell ref="E2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="Q4:U4"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="Q6:U6"/>
-    <mergeCell ref="Q7:U7"/>
-    <mergeCell ref="Q8:U8"/>
-    <mergeCell ref="Q9:U9"/>
-    <mergeCell ref="Q10:U10"/>
-    <mergeCell ref="Q12:U12"/>
-    <mergeCell ref="Q13:U13"/>
-    <mergeCell ref="Q14:U14"/>
-    <mergeCell ref="Q15:U15"/>
-    <mergeCell ref="Q16:U16"/>
-    <mergeCell ref="Q35:U35"/>
-    <mergeCell ref="Q27:U27"/>
-    <mergeCell ref="Q28:U28"/>
-    <mergeCell ref="Q29:U29"/>
-    <mergeCell ref="Q30:U30"/>
-    <mergeCell ref="Q31:U31"/>
-    <mergeCell ref="Q32:U32"/>
-    <mergeCell ref="Q33:U33"/>
-    <mergeCell ref="Q34:U34"/>
+    <mergeCell ref="Q48:U48"/>
+    <mergeCell ref="Q49:U49"/>
+    <mergeCell ref="Q50:U50"/>
+    <mergeCell ref="Q51:U51"/>
+    <mergeCell ref="Q52:U52"/>
     <mergeCell ref="Q47:U47"/>
     <mergeCell ref="Q36:U36"/>
     <mergeCell ref="Q38:U38"/>
@@ -2567,11 +2666,31 @@
     <mergeCell ref="Q44:U44"/>
     <mergeCell ref="Q45:U45"/>
     <mergeCell ref="Q46:U46"/>
-    <mergeCell ref="Q48:U48"/>
-    <mergeCell ref="Q49:U49"/>
-    <mergeCell ref="Q50:U50"/>
-    <mergeCell ref="Q51:U51"/>
-    <mergeCell ref="Q52:U52"/>
+    <mergeCell ref="Q35:U35"/>
+    <mergeCell ref="Q27:U27"/>
+    <mergeCell ref="Q28:U28"/>
+    <mergeCell ref="Q29:U29"/>
+    <mergeCell ref="Q30:U30"/>
+    <mergeCell ref="Q31:U31"/>
+    <mergeCell ref="Q32:U32"/>
+    <mergeCell ref="Q33:U33"/>
+    <mergeCell ref="Q34:U34"/>
+    <mergeCell ref="Q12:U12"/>
+    <mergeCell ref="Q13:U13"/>
+    <mergeCell ref="Q14:U14"/>
+    <mergeCell ref="Q15:U15"/>
+    <mergeCell ref="Q16:U16"/>
+    <mergeCell ref="Q11:U11"/>
+    <mergeCell ref="E2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="Q6:U6"/>
+    <mergeCell ref="Q7:U7"/>
+    <mergeCell ref="Q8:U8"/>
+    <mergeCell ref="Q9:U9"/>
+    <mergeCell ref="Q10:U10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>